<commit_message>
FIX: Correct CSV tests to use new response codes
</commit_message>
<xml_diff>
--- a/test_files/csv_test_files/COS10001-Tasks.xlsx
+++ b/test_files/csv_test_files/COS10001-Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keshavkatarya/doubtfire-api/test_files/submissions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acain/Documents/Code/GitHub/doubtfire-api/test_files/csv_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD916F46-EA1C-7949-B5D5-7B24EAA510BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AA0691-77D8-0E45-89AB-1997F2887694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -91,17 +91,20 @@
     <t>Mon</t>
   </si>
   <si>
-    <t>Assignment 12</t>
-  </si>
-  <si>
-    <t>A12</t>
+    <t>NEWTD1</t>
+  </si>
+  <si>
+    <t>New Task Def 1</t>
+  </si>
+  <si>
+    <t>tutorial_stream</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -935,15 +938,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -998,13 +1001,16 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>

</xml_diff>